<commit_message>
exception and boolean handling.
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12146\Desktop\Kickin Tech\xlsx-to-sql-parser\xlsx-to-sql-parser-main\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12146\Desktop\Kickin Tech\xlsx-to-sql-converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E45C8DAD-21E7-47FA-B951-C552D2D3B3D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA19CD02-229B-4A6B-9F24-FFD75ADE6966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{7D5F7947-847E-4F2B-A683-CC925C25956F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="67">
   <si>
     <t>L:0001</t>
   </si>
@@ -126,12 +126,6 @@
   </si>
   <si>
     <t>L:0030</t>
-  </si>
-  <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>POTATO</t>
   </si>
   <si>
     <t>L:0031</t>
@@ -284,8 +278,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -602,419 +597,422 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0476389-7B6D-4DE4-A236-F4BE280B9469}">
   <dimension ref="B1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
+    <col min="2" max="2" width="23.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.7265625" style="1"/>
+    <col min="5" max="5" width="30.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B1">
+      <c r="B1" s="1">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
+      <c r="D6" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="G5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B6" t="s">
+      <c r="D7" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
+      <c r="D8" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
+      <c r="D9" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B9" t="s">
+      <c r="D10" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B10" t="s">
+      <c r="D11" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B11" t="s">
+      <c r="D12" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
+      <c r="D13" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+      <c r="D14" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D13" t="b">
-        <v>0</v>
-      </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B14" t="s">
+      <c r="D15" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D14" t="b">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+      <c r="D16" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B17" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-      <c r="G15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B16" t="s">
+      <c r="D17" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D16" t="b">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="D18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
+      <c r="D19" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D18" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
+      <c r="D20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B21" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
+      <c r="D21" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" t="s">
+      <c r="D22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B23" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D21" t="b">
-        <v>0</v>
-      </c>
-      <c r="E21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="D23" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B24" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D22" t="b">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+      <c r="D24" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="D25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B26" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="D24" t="b">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
+      <c r="D26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
+      <c r="D27" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+      <c r="D28" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B29" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D27" t="b">
-        <v>0</v>
-      </c>
-      <c r="G27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
+      <c r="D29" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B30" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D28" t="b">
-        <v>1</v>
-      </c>
-      <c r="G28" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+      <c r="D30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B31" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D29" t="b">
-        <v>0</v>
-      </c>
-      <c r="G29" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
+      <c r="D31" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D30" t="b">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" t="s">
+      <c r="D32" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D31" t="b">
-        <v>0</v>
-      </c>
-      <c r="G31" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" t="s">
+      <c r="D33" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B34" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B33" t="s">
+      <c r="D34" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D33" t="b">
-        <v>0</v>
-      </c>
-      <c r="G33" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" t="s">
+      <c r="D35" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D34" t="b">
-        <v>1</v>
-      </c>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="G34" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D35" t="s">
-        <v>30</v>
-      </c>
-      <c r="G35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D36" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="G36" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>